<commit_message>
Missing imports fixed - xmltodict - jsonpickle - docutils - pillow
</commit_message>
<xml_diff>
--- a/testMap.xlsx
+++ b/testMap.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Pens" sheetId="1" state="visible" r:id="rId3"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="17">
   <si>
     <t xml:space="preserve">Objects' name</t>
   </si>
@@ -62,6 +62,12 @@
   </si>
   <si>
     <t xml:space="preserve">Teszt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">joistNames</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PS8 (202mm)</t>
   </si>
   <si>
     <t xml:space="preserve">AC_show2DHotspotsIn3D</t>
@@ -284,7 +290,7 @@
   <dimension ref="E1:K2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -349,7 +355,7 @@
   <dimension ref="E1:K2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -358,7 +364,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="19.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="11.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="8.95"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="1" width="11.53"/>
@@ -414,7 +420,7 @@
   <dimension ref="E1:K2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -477,7 +483,7 @@
   <dimension ref="E1:K5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -486,7 +492,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="19.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="11.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="8.95"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="1" width="11.53"/>
@@ -563,20 +569,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="E1:K2"/>
+  <dimension ref="E1:K3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="1:1048576"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="25.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="19.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="8.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="11.44"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="8.95"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="1" width="11.53"/>
   </cols>
@@ -610,6 +616,14 @@
       </c>
       <c r="J2" s="1" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -631,7 +645,7 @@
   <dimension ref="E1:K2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -640,7 +654,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="23.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="19.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="11.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="8.95"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="1" width="11.53"/>
@@ -671,7 +685,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F2" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J2" s="1" t="n">
         <v>1</v>
@@ -695,8 +709,8 @@
   </sheetPr>
   <dimension ref="E1:K3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="1:1048576"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -705,7 +719,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="19.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="11.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="8.95"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="1" width="11.53"/>
@@ -736,7 +750,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F2" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J2" s="1" t="n">
         <v>248</v>
@@ -744,7 +758,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G3" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J3" s="1" t="n">
         <v>247</v>

</xml_diff>